<commit_message>
As far as I got on my own
</commit_message>
<xml_diff>
--- a/Project0/DataSpreadsheet/RoSADatasheet.xlsx
+++ b/Project0/DataSpreadsheet/RoSADatasheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Eggs</t>
   </si>
@@ -208,6 +208,21 @@
   </si>
   <si>
     <t>aurelianderu@EBI.com</t>
+  </si>
+  <si>
+    <t>Imara Gimura</t>
+  </si>
+  <si>
+    <t>imarasnakeeyes@EBI.com</t>
+  </si>
+  <si>
+    <t>Zelda BOTW (5% Discount)</t>
+  </si>
+  <si>
+    <t>Vincent Pryor</t>
+  </si>
+  <si>
+    <t>DrPryor@EBI.com</t>
   </si>
 </sst>
 </file>
@@ -716,7 +731,7 @@
         <v>39.99</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -742,7 +757,7 @@
         <v>899.99</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -873,7 +888,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -960,6 +975,22 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -973,7 +1004,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -1057,6 +1088,34 @@
         <v>33.25</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>189.95249999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>4499.95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>